<commit_message>
change source tr tv refactor enveloppe ecs finished
</commit_message>
<xml_diff>
--- a/data_processing_cstb/traitement_donnees_metier/assets/DT_TMA_DPE_Tables_de_références_v1.3.1.xlsx
+++ b/data_processing_cstb/traitement_donnees_metier/assets/DT_TMA_DPE_Tables_de_références_v1.3.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cstbdata\MONWORKSPACE\Gitlab\de-dpe-processing\data_processing_cstb\traitement_donnees_metier\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4437566E-571F-4444-B9E9-51C8098BCB7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB54D6-6910-4993-B324-D1FC44A40632}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" tabRatio="868" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versioning" sheetId="69" r:id="rId1"/>
@@ -9765,8 +9765,8 @@
   <sheetPr codeName="Feuil16"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13599,8 +13599,8 @@
   <sheetPr codeName="Feuil6"/>
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14846,7 +14846,7 @@
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17384,6 +17384,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010070A8FD186B68324BB79A5C37EC99AB72" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e49ea6d43c913324368c5e38e1ba174b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dc7b3e59-32ff-407d-b161-fa25a3f51fe5" xmlns:ns3="375630ec-ac37-4b9f-9710-43e3a6e12605" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b9196580bd2f30d094debb531bcb1b7" ns2:_="" ns3:_="">
     <xsd:import namespace="dc7b3e59-32ff-407d-b161-fa25a3f51fe5"/>
@@ -17586,22 +17601,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{616E3892-A826-4EAB-93B6-BABD219D84DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A375065D-B86D-4878-A597-E1CEE74F891B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A52F9A9-A1FE-4D57-AD95-68D910F5C281}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17618,21 +17635,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{616E3892-A826-4EAB-93B6-BABD219D84DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A375065D-B86D-4878-A597-E1CEE74F891B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>